<commit_message>
Added piston test module, TODO: change other ymls + implement, test
</commit_message>
<xml_diff>
--- a/Server_files/plugins/ProjectXXX/Module_Coordinates.xlsx
+++ b/Server_files/plugins/ProjectXXX/Module_Coordinates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="16">
   <si>
     <t>Raum mit Säulen</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t>passageWay std, straight, redstone door</t>
+  </si>
+  <si>
+    <t>passageWay Piston test</t>
+  </si>
+  <si>
+    <t>door redst exit</t>
+  </si>
+  <si>
+    <t>door redst entry</t>
   </si>
 </sst>
 </file>
@@ -449,15 +458,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:Y23"/>
+  <dimension ref="C3:AE27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="AA14" sqref="AA14"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AF30" sqref="AF30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="27" max="27" width="16.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
@@ -486,8 +498,15 @@
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
-    </row>
-    <row r="5" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="5"/>
+      <c r="AE3" s="5"/>
+    </row>
+    <row r="5" spans="3:31" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>2</v>
       </c>
@@ -510,8 +529,14 @@
       <c r="W5" s="2">
         <v>1117</v>
       </c>
-    </row>
-    <row r="6" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AB5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC5" s="2">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="6" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
@@ -550,8 +575,18 @@
         <v>64</v>
       </c>
       <c r="X6" s="3"/>
-    </row>
-    <row r="7" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC6" s="2">
+        <v>78</v>
+      </c>
+      <c r="AD6" s="3"/>
+    </row>
+    <row r="7" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" t="s">
         <v>4</v>
@@ -578,14 +613,22 @@
       <c r="W7" s="2">
         <v>-183</v>
       </c>
-    </row>
-    <row r="8" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA7" s="1"/>
+      <c r="AB7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC7" s="2">
+        <v>-244</v>
+      </c>
+    </row>
+    <row r="8" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="I8" s="1"/>
       <c r="O8" s="1"/>
       <c r="U8" s="1"/>
-    </row>
-    <row r="9" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA8" s="1"/>
+    </row>
+    <row r="9" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="D9" t="s">
         <v>2</v>
@@ -628,8 +671,19 @@
         <f>W9-W$5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA9" s="1"/>
+      <c r="AB9" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC9" s="2">
+        <v>1128</v>
+      </c>
+      <c r="AE9" s="4">
+        <f>AC9-AC$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
@@ -692,8 +746,24 @@
         <f>W10-W$6</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC10" s="2">
+        <v>82</v>
+      </c>
+      <c r="AD10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE10" s="4">
+        <f>AC10-AC$6</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="D11" t="s">
         <v>4</v>
@@ -736,14 +806,26 @@
         <f>W11-W$7</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA11" s="1"/>
+      <c r="AB11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC11" s="2">
+        <v>-241</v>
+      </c>
+      <c r="AE11" s="4">
+        <f>AC11-AC$7</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="I12" s="1"/>
       <c r="O12" s="1"/>
       <c r="U12" s="1"/>
-    </row>
-    <row r="13" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA12" s="1"/>
+    </row>
+    <row r="13" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="D13" t="s">
         <v>2</v>
@@ -786,8 +868,19 @@
         <f>W13-W$5</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA13" s="1"/>
+      <c r="AB13" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC13" s="2">
+        <v>1140</v>
+      </c>
+      <c r="AE13" s="4">
+        <f>AC13-AC$5</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
@@ -850,8 +943,24 @@
         <f>W14-W$6</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC14" s="2">
+        <v>82</v>
+      </c>
+      <c r="AD14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE14" s="4">
+        <f>AC14-AC$6</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" t="s">
         <v>4</v>
@@ -894,14 +1003,26 @@
         <f>W15-W$7</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA15" s="1"/>
+      <c r="AB15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC15" s="2">
+        <v>-241</v>
+      </c>
+      <c r="AE15" s="4">
+        <f>AC15-AC$7</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="I16" s="1"/>
       <c r="O16" s="1"/>
       <c r="U16" s="1"/>
-    </row>
-    <row r="17" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA16" s="1"/>
+    </row>
+    <row r="17" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" t="s">
         <v>2</v>
@@ -941,8 +1062,18 @@
         <f>W17-W$5</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AB17" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC17" s="2">
+        <v>1134</v>
+      </c>
+      <c r="AE17" s="4">
+        <f>AC17-AC$5</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1005,8 +1136,24 @@
         <f>W18-W$6</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC18" s="2">
+        <v>82</v>
+      </c>
+      <c r="AD18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE18" s="4">
+        <f>AC18-AC$6</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" t="s">
         <v>4</v>
@@ -1046,11 +1193,21 @@
         <f>W19-W$7</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AB19" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC19" s="2">
+        <v>-242</v>
+      </c>
+      <c r="AE19" s="4">
+        <f>AC19-AC$7</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" t="s">
         <v>2</v>
@@ -1062,8 +1219,18 @@
         <f>E21-E$5</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AB21" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC21" s="2">
+        <v>1132</v>
+      </c>
+      <c r="AE21" s="4">
+        <f>AC21-AC$5</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>8</v>
       </c>
@@ -1081,8 +1248,24 @@
         <v>1</v>
       </c>
       <c r="L22" s="3"/>
-    </row>
-    <row r="23" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC22" s="2">
+        <v>82</v>
+      </c>
+      <c r="AD22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE22" s="4">
+        <f>AC22-AC$6</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="3:31" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>4</v>
       </c>
@@ -1093,13 +1276,66 @@
         <f>E23-E$7</f>
         <v>5</v>
       </c>
+      <c r="AB23" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC23" s="2">
+        <v>-235</v>
+      </c>
+      <c r="AE23" s="4">
+        <f>AC23-AC$7</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="3:31" x14ac:dyDescent="0.25">
+      <c r="AB25" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC25" s="2">
+        <v>1136</v>
+      </c>
+      <c r="AE25" s="4">
+        <f>AC25-AC$5</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="3:31" x14ac:dyDescent="0.25">
+      <c r="AA26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC26" s="2">
+        <v>82</v>
+      </c>
+      <c r="AD26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE26" s="4">
+        <f>AC26-AC$6</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="3:31" x14ac:dyDescent="0.25">
+      <c r="AB27" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC27" s="2">
+        <v>-235</v>
+      </c>
+      <c r="AE27" s="4">
+        <f>AC27-AC$7</f>
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="U3:Y3"/>
     <mergeCell ref="O3:S3"/>
     <mergeCell ref="I3:M3"/>
     <mergeCell ref="C3:G3"/>
+    <mergeCell ref="AA3:AE3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
added and tested falling type doors
</commit_message>
<xml_diff>
--- a/Server_files/plugins/ProjectXXX/Module_Coordinates.xlsx
+++ b/Server_files/plugins/ProjectXXX/Module_Coordinates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="17">
   <si>
     <t>Raum mit Säulen</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>door redst entry</t>
+  </si>
+  <si>
+    <t>passageWay Falling test</t>
   </si>
 </sst>
 </file>
@@ -458,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:AE27"/>
+  <dimension ref="C3:AK27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AF30" sqref="AF30"/>
+      <selection activeCell="AJ26" sqref="AJ26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,7 +472,7 @@
     <col min="27" max="27" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
@@ -505,8 +508,15 @@
       <c r="AC3" s="5"/>
       <c r="AD3" s="5"/>
       <c r="AE3" s="5"/>
-    </row>
-    <row r="5" spans="3:31" x14ac:dyDescent="0.25">
+      <c r="AG3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH3" s="5"/>
+      <c r="AI3" s="5"/>
+      <c r="AJ3" s="5"/>
+      <c r="AK3" s="5"/>
+    </row>
+    <row r="5" spans="3:37" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>2</v>
       </c>
@@ -535,8 +545,14 @@
       <c r="AC5" s="2">
         <v>1128</v>
       </c>
-    </row>
-    <row r="6" spans="3:31" x14ac:dyDescent="0.25">
+      <c r="AH5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI5" s="2">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="6" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
@@ -585,8 +601,18 @@
         <v>78</v>
       </c>
       <c r="AD6" s="3"/>
-    </row>
-    <row r="7" spans="3:31" x14ac:dyDescent="0.25">
+      <c r="AG6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI6" s="2">
+        <v>78</v>
+      </c>
+      <c r="AJ6" s="3"/>
+    </row>
+    <row r="7" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" t="s">
         <v>4</v>
@@ -620,15 +646,23 @@
       <c r="AC7" s="2">
         <v>-244</v>
       </c>
-    </row>
-    <row r="8" spans="3:31" x14ac:dyDescent="0.25">
+      <c r="AG7" s="1"/>
+      <c r="AH7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI7" s="2">
+        <v>-223</v>
+      </c>
+    </row>
+    <row r="8" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="I8" s="1"/>
       <c r="O8" s="1"/>
       <c r="U8" s="1"/>
       <c r="AA8" s="1"/>
-    </row>
-    <row r="9" spans="3:31" x14ac:dyDescent="0.25">
+      <c r="AG8" s="1"/>
+    </row>
+    <row r="9" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="D9" t="s">
         <v>2</v>
@@ -682,8 +716,19 @@
         <f>AC9-AC$5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="3:31" x14ac:dyDescent="0.25">
+      <c r="AG9" s="1"/>
+      <c r="AH9" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI9" s="2">
+        <v>1131</v>
+      </c>
+      <c r="AK9" s="4">
+        <f>AI9-AI$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
@@ -762,8 +807,24 @@
         <f>AC10-AC$6</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="3:31" x14ac:dyDescent="0.25">
+      <c r="AG10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI10" s="2">
+        <v>82</v>
+      </c>
+      <c r="AJ10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AK10" s="4">
+        <f>AI10-AI$6</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="D11" t="s">
         <v>4</v>
@@ -817,15 +878,27 @@
         <f>AC11-AC$7</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="3:31" x14ac:dyDescent="0.25">
+      <c r="AG11" s="1"/>
+      <c r="AH11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI11" s="2">
+        <v>-220</v>
+      </c>
+      <c r="AK11" s="4">
+        <f>AI11-AI$7</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="I12" s="1"/>
       <c r="O12" s="1"/>
       <c r="U12" s="1"/>
       <c r="AA12" s="1"/>
-    </row>
-    <row r="13" spans="3:31" x14ac:dyDescent="0.25">
+      <c r="AG12" s="1"/>
+    </row>
+    <row r="13" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="D13" t="s">
         <v>2</v>
@@ -879,8 +952,19 @@
         <f>AC13-AC$5</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="3:31" x14ac:dyDescent="0.25">
+      <c r="AG13" s="1"/>
+      <c r="AH13" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI13" s="2">
+        <v>1143</v>
+      </c>
+      <c r="AK13" s="4">
+        <f>AI13-AI$5</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
@@ -959,8 +1043,24 @@
         <f>AC14-AC$6</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="3:31" x14ac:dyDescent="0.25">
+      <c r="AG14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI14" s="2">
+        <v>82</v>
+      </c>
+      <c r="AJ14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AK14" s="4">
+        <f>AI14-AI$6</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" t="s">
         <v>4</v>
@@ -1014,15 +1114,27 @@
         <f>AC15-AC$7</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="3:31" x14ac:dyDescent="0.25">
+      <c r="AG15" s="1"/>
+      <c r="AH15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI15" s="2">
+        <v>-220</v>
+      </c>
+      <c r="AK15" s="4">
+        <f>AI15-AI$7</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="I16" s="1"/>
       <c r="O16" s="1"/>
       <c r="U16" s="1"/>
       <c r="AA16" s="1"/>
-    </row>
-    <row r="17" spans="3:31" x14ac:dyDescent="0.25">
+      <c r="AG16" s="1"/>
+    </row>
+    <row r="17" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" t="s">
         <v>2</v>
@@ -1072,8 +1184,18 @@
         <f>AC17-AC$5</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="3:31" x14ac:dyDescent="0.25">
+      <c r="AH17" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI17" s="2">
+        <v>1137</v>
+      </c>
+      <c r="AK17" s="4">
+        <f>AI17-AI$5</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1152,8 +1274,24 @@
         <f>AC18-AC$6</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="3:31" x14ac:dyDescent="0.25">
+      <c r="AG18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI18" s="2">
+        <v>82</v>
+      </c>
+      <c r="AJ18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AK18" s="4">
+        <f>AI18-AI$6</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" t="s">
         <v>4</v>
@@ -1203,11 +1341,21 @@
         <f>AC19-AC$7</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="3:31" x14ac:dyDescent="0.25">
+      <c r="AH19" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI19" s="2">
+        <v>-219</v>
+      </c>
+      <c r="AK19" s="4">
+        <f>AI19-AI$7</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="3:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" t="s">
         <v>2</v>
@@ -1230,7 +1378,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="3:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>8</v>
       </c>
@@ -1264,8 +1412,9 @@
         <f>AC22-AC$6</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="3:31" x14ac:dyDescent="0.25">
+      <c r="AJ22" s="3"/>
+    </row>
+    <row r="23" spans="3:37" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>4</v>
       </c>
@@ -1287,7 +1436,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="3:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:37" x14ac:dyDescent="0.25">
       <c r="AB25" t="s">
         <v>2</v>
       </c>
@@ -1299,7 +1448,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="3:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:37" x14ac:dyDescent="0.25">
       <c r="AA26" s="1" t="s">
         <v>14</v>
       </c>
@@ -1316,8 +1465,9 @@
         <f>AC26-AC$6</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="3:31" x14ac:dyDescent="0.25">
+      <c r="AJ26" s="3"/>
+    </row>
+    <row r="27" spans="3:37" x14ac:dyDescent="0.25">
       <c r="AB27" t="s">
         <v>4</v>
       </c>
@@ -1330,7 +1480,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="AG3:AK3"/>
     <mergeCell ref="U3:Y3"/>
     <mergeCell ref="O3:S3"/>
     <mergeCell ref="I3:M3"/>

</xml_diff>